<commit_message>
Removed seperate web parts for managing timesheet. Now managing timesheet in single webpart for add,update,delete and view. Added repository pattern.
</commit_message>
<xml_diff>
--- a/TestPlan/TestPlan.xlsx
+++ b/TestPlan/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SumitM\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AF24E2-1202-4F34-A80F-464E3D7E10F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E69931-88AB-437D-9C2A-9E31CA0927C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,16 +252,16 @@
     <t>User is getting selected timesheet details.</t>
   </si>
   <si>
-    <t>User should get "Back" button on view timesheet page.</t>
-  </si>
-  <si>
-    <t>User is getting get "Back" button on view timesheet page.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing page by clicking on "Back" button.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to timesheet listing page by clicking on "Back" button.</t>
+    <t>User is getting redirected to timesheet listing page by clicking on "Cancel" button.</t>
+  </si>
+  <si>
+    <t>User should be redirected to timesheet listing page by clicking on "Cancel" button.</t>
+  </si>
+  <si>
+    <t>User should get "Cancel" button on timesheet page.</t>
+  </si>
+  <si>
+    <t>User is getting get "Cancel" button on timesheet page.</t>
   </si>
 </sst>
 </file>
@@ -930,7 +930,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,24 +1258,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove timesheet listing webpart. Now timesheet listing and crud operations will be handled by single webpart. Also Reading listname from web.config file.
</commit_message>
<xml_diff>
--- a/TestPlan/TestPlan.xlsx
+++ b/TestPlan/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SumitM\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E69931-88AB-437D-9C2A-9E31CA0927C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C1B79C-37C5-4199-A9A8-BC1A113154CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t>Module</t>
   </si>
@@ -81,15 +81,6 @@
     <t>Timesheet should be created and user should be notified for new timesheet creation.</t>
   </si>
   <si>
-    <t>User should be redirected to timesheet listing page after successfully creating new timesheet.</t>
-  </si>
-  <si>
-    <t>New timesheet should be created and user should be redirected to timesheet listing page.</t>
-  </si>
-  <si>
-    <t>Timesheet is getting created and user is getting redirected to timesheet listing page.</t>
-  </si>
-  <si>
     <t>User should not be able to create new timesheet without selecting valid category.</t>
   </si>
   <si>
@@ -108,15 +99,6 @@
     <t>New timesheet should be created.</t>
   </si>
   <si>
-    <t>User should be redirected to timesheet listing page by clicking on cancel button.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing page.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to timesheet listing page.</t>
-  </si>
-  <si>
     <t>Edit Timesheet</t>
   </si>
   <si>
@@ -138,15 +120,6 @@
     <t>Timesheet is getting updated and user is getting message "Timesheet Updated..!".</t>
   </si>
   <si>
-    <t>User should be redirected to timesheet listing page after successfully updating timesheet.</t>
-  </si>
-  <si>
-    <t>Timesheet should be updated and user should be redirected to timesheet listing page.</t>
-  </si>
-  <si>
-    <t>Timesheet is getting updated and user is getting redirected to timesheet listing page.</t>
-  </si>
-  <si>
     <t>User should not be able to update timesheet without selecting valid category.</t>
   </si>
   <si>
@@ -192,27 +165,6 @@
     <t>Users is getting options to view, edit and delete existing timesheets.</t>
   </si>
   <si>
-    <t>User should be redirected to view timesheet page by clicking on "View" option and get selected timesheet details to view.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to view timesheet page by clicking on "View" option and getting selected timesheet details to view.</t>
-  </si>
-  <si>
-    <t>User should be redirected to edit timesheet page by clicking on "Edit" option and get "Submit" button to update timesheet along with correct timesheet details.</t>
-  </si>
-  <si>
-    <t>User should be redirected to eidt timesheet page by clicking on "Edit" option and get "Submit" button to update timesheet along with correct timesheet details.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to edit timesheet page by clicking on "Edit" option and getting "Submit" button to update timesheet along with correct timesheet details.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to edit timesheet page by clicking on "Delete" option and getting "Delete" button to delete timesheet along with correct timesheet details.</t>
-  </si>
-  <si>
-    <t>User should be redirected to edit timesheet page by clicking on "Delete" option and get "Delete" button to delete timesheet along with correct timesheet details.</t>
-  </si>
-  <si>
     <t>Paging should be displayed to view timesheet details on next page.</t>
   </si>
   <si>
@@ -234,12 +186,6 @@
     <t>Delete Timesheet</t>
   </si>
   <si>
-    <t>User should be redirected to timesheet listing page after succcessfully deleting timsheet.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to timesheet listing page after succcessfully deleting timsheet.</t>
-  </si>
-  <si>
     <t>User should be notified for successfully deletion of timesheet.</t>
   </si>
   <si>
@@ -252,16 +198,88 @@
     <t>User is getting selected timesheet details.</t>
   </si>
   <si>
-    <t>User is getting redirected to timesheet listing page by clicking on "Cancel" button.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing page by clicking on "Cancel" button.</t>
-  </si>
-  <si>
-    <t>User should get "Cancel" button on timesheet page.</t>
-  </si>
-  <si>
-    <t>User is getting get "Cancel" button on timesheet page.</t>
+    <t>User should be redirected to timesheet listing by clicking on cancel button.</t>
+  </si>
+  <si>
+    <t>User should be redirected to timesheet listing.</t>
+  </si>
+  <si>
+    <t>User is getting redirected to timesheet listing.</t>
+  </si>
+  <si>
+    <t>User should get "New Entry" link to create new timesheet entry.</t>
+  </si>
+  <si>
+    <t>User is getting "New Entry" link to create new timesheet entry.</t>
+  </si>
+  <si>
+    <t>User should get timesheet to edit by clicking on "Edit" option and get "Submit" button to update timesheet along with correct timesheet details.</t>
+  </si>
+  <si>
+    <t>User is getting timesheet to edit by clicking on "Edit" option and get "Submit" button to update timesheet along with correct timesheet details.</t>
+  </si>
+  <si>
+    <t>User should be confirmation message by clicking on "Delete" option to delete particular timesheet entry.</t>
+  </si>
+  <si>
+    <t>User is getting confirmation message by clicking on "Delete" option to delete particular timesheet entry.</t>
+  </si>
+  <si>
+    <t>On delete confirmatin message, timesheet entry should be deleted if user clicks on Ok Button and user should get message like "Timesheet entry deleted..!"</t>
+  </si>
+  <si>
+    <t>Timesheet is getting deleted by clicking on OK button of confirmation dialogue box and getting message like "Timesheet entry deleted..!".</t>
+  </si>
+  <si>
+    <t>On delete confirmatin dialogue, timesheet entry should be deleted if user clicks on Ok Button and user should get message like "Timesheet entry deleted..!"</t>
+  </si>
+  <si>
+    <t>On delete confirmatin dialogue, timesheet entry should not be deleted if user clicks on Cancel Button.</t>
+  </si>
+  <si>
+    <t>On delete confirmatin dialogue, timesheet entry is not getting deleted if user clicks on Cancel Button.</t>
+  </si>
+  <si>
+    <t>User is getting redirected to timesheet listing after succcessfully deleting timsheet and getting updated timesheet records.</t>
+  </si>
+  <si>
+    <t>User should be redirected to timesheet listing after succcessfully deleting timsheet and get updated timesheet records.</t>
+  </si>
+  <si>
+    <t>User should be redirected to timesheet listing by clicking on "Back" button.</t>
+  </si>
+  <si>
+    <t>User should get "Back" button on view timesheet.</t>
+  </si>
+  <si>
+    <t>User is getting "Back" button on view timesheet.</t>
+  </si>
+  <si>
+    <t>User should be redirected to timesheet listing after successfully creating new timesheet.</t>
+  </si>
+  <si>
+    <t>New timesheet should be created and user should be redirected to timesheet listing.</t>
+  </si>
+  <si>
+    <t>User should be redirected to timesheet listing after successfully updating timesheet.</t>
+  </si>
+  <si>
+    <t>User should be redirected to view timesheet by clicking on "View" option and get selected timesheet details to view.</t>
+  </si>
+  <si>
+    <t>User is getting redirected to timesheet listing by clicking on "Back" button.</t>
+  </si>
+  <si>
+    <t>Timesheet is getting created and user is getting redirected to timesheet listing.</t>
+  </si>
+  <si>
+    <t>Timesheet should be updated and user should be redirected to timesheet listing.</t>
+  </si>
+  <si>
+    <t>Timesheet is getting updated and user is getting redirected to timesheet listing.</t>
+  </si>
+  <si>
+    <t>User is getting redirected to view timesheet by clicking on "View" option and getting selected timesheet details to view.</t>
   </si>
 </sst>
 </file>
@@ -927,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +1006,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1004,51 +1022,51 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -1073,209 +1091,242 @@
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>73</v>
+      <c r="D36" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Display timesheets in descending order of timesheet date and updated test plan
</commit_message>
<xml_diff>
--- a/TestPlan/TestPlan.xlsx
+++ b/TestPlan/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SumitM\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C1B79C-37C5-4199-A9A8-BC1A113154CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC6A2F3-E890-4156-944C-C326677E29A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,8 @@
     <sheet name="Timesheet List" sheetId="2" r:id="rId2"/>
     <sheet name="Add New Timesheet" sheetId="3" r:id="rId3"/>
     <sheet name="Edit Timesheet" sheetId="4" r:id="rId4"/>
-    <sheet name="Delete Timesheet" sheetId="5" r:id="rId5"/>
-    <sheet name="View Timesheet" sheetId="6" r:id="rId6"/>
-    <sheet name="SharePoint Timesheet List" sheetId="7" r:id="rId7"/>
+    <sheet name="View Timesheet" sheetId="6" r:id="rId5"/>
+    <sheet name="SharePoint Timesheet List" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
   <si>
     <t>Module</t>
   </si>
@@ -39,9 +38,6 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>Add Timesheet</t>
-  </si>
-  <si>
     <t>User should not enter invalid timesheet date.</t>
   </si>
   <si>
@@ -186,108 +182,113 @@
     <t>Delete Timesheet</t>
   </si>
   <si>
-    <t>User should be notified for successfully deletion of timesheet.</t>
-  </si>
-  <si>
-    <t>User is getting notification for timesheet deleted.</t>
-  </si>
-  <si>
-    <t>User should get selected timesheet details.</t>
-  </si>
-  <si>
-    <t>User is getting selected timesheet details.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing by clicking on cancel button.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to timesheet listing.</t>
-  </si>
-  <si>
     <t>User should get "New Entry" link to create new timesheet entry.</t>
   </si>
   <si>
     <t>User is getting "New Entry" link to create new timesheet entry.</t>
   </si>
   <si>
-    <t>User should get timesheet to edit by clicking on "Edit" option and get "Submit" button to update timesheet along with correct timesheet details.</t>
-  </si>
-  <si>
-    <t>User is getting timesheet to edit by clicking on "Edit" option and get "Submit" button to update timesheet along with correct timesheet details.</t>
-  </si>
-  <si>
-    <t>User should be confirmation message by clicking on "Delete" option to delete particular timesheet entry.</t>
-  </si>
-  <si>
     <t>User is getting confirmation message by clicking on "Delete" option to delete particular timesheet entry.</t>
   </si>
   <si>
-    <t>On delete confirmatin message, timesheet entry should be deleted if user clicks on Ok Button and user should get message like "Timesheet entry deleted..!"</t>
-  </si>
-  <si>
-    <t>Timesheet is getting deleted by clicking on OK button of confirmation dialogue box and getting message like "Timesheet entry deleted..!".</t>
-  </si>
-  <si>
-    <t>On delete confirmatin dialogue, timesheet entry should be deleted if user clicks on Ok Button and user should get message like "Timesheet entry deleted..!"</t>
-  </si>
-  <si>
-    <t>On delete confirmatin dialogue, timesheet entry should not be deleted if user clicks on Cancel Button.</t>
-  </si>
-  <si>
-    <t>On delete confirmatin dialogue, timesheet entry is not getting deleted if user clicks on Cancel Button.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to timesheet listing after succcessfully deleting timsheet and getting updated timesheet records.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing after succcessfully deleting timsheet and get updated timesheet records.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing by clicking on "Back" button.</t>
-  </si>
-  <si>
-    <t>User should get "Back" button on view timesheet.</t>
-  </si>
-  <si>
-    <t>User is getting "Back" button on view timesheet.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing after successfully creating new timesheet.</t>
-  </si>
-  <si>
-    <t>New timesheet should be created and user should be redirected to timesheet listing.</t>
-  </si>
-  <si>
-    <t>User should be redirected to timesheet listing after successfully updating timesheet.</t>
-  </si>
-  <si>
-    <t>User should be redirected to view timesheet by clicking on "View" option and get selected timesheet details to view.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to timesheet listing by clicking on "Back" button.</t>
-  </si>
-  <si>
-    <t>Timesheet is getting created and user is getting redirected to timesheet listing.</t>
-  </si>
-  <si>
-    <t>Timesheet should be updated and user should be redirected to timesheet listing.</t>
-  </si>
-  <si>
-    <t>Timesheet is getting updated and user is getting redirected to timesheet listing.</t>
-  </si>
-  <si>
-    <t>User is getting redirected to view timesheet by clicking on "View" option and getting selected timesheet details to view.</t>
+    <t>Timesheet entry should be deleted if user clicks on Ok Button on confirmation dialogue box and user should be notified with message "Timesheet entry deleted..!"</t>
+  </si>
+  <si>
+    <t>Timesheet entry is getting deleted when user clicks on Ok Button on confirmation dialogue box and user is getting notified with message "Timesheet entry deleted..!"</t>
+  </si>
+  <si>
+    <t>User should get timesheet listing screen after succcessfully deletion of timsheet and get updated timesheet records.</t>
+  </si>
+  <si>
+    <t>User is getting timesheet listing screen after succcessfully deletion of timsheet and getings updated timesheet records.</t>
+  </si>
+  <si>
+    <t>Timesheet entry should not be deleted if user clicks Cancel Button on confirmation dialogue box.</t>
+  </si>
+  <si>
+    <t>Timesheet entry is not getting deleted if user clicks Cancel Button on confirmation dialogue box.</t>
+  </si>
+  <si>
+    <t>New Timesheet</t>
+  </si>
+  <si>
+    <t>User should get view timesheet screen by clicking on "View" option.</t>
+  </si>
+  <si>
+    <t>User is getting view timesheet screen by clicking on "View" option.</t>
+  </si>
+  <si>
+    <t>User should get edit timesheet screen by clicking on "Edit" option.</t>
+  </si>
+  <si>
+    <t>User is getting edit timesheet screen by clicking on "Edit" option.</t>
+  </si>
+  <si>
+    <t>User should get correct timesheet details for selected timesheet entry.</t>
+  </si>
+  <si>
+    <t>User is getting correct timesheet details for selected timesheet entry.</t>
+  </si>
+  <si>
+    <t>User should get "Back" button on view timesheet screen.</t>
+  </si>
+  <si>
+    <t>User is getting "Back" button on view timesheet screen.</t>
+  </si>
+  <si>
+    <t>User should get timesheet listing screen by clicking on "Back" button.</t>
+  </si>
+  <si>
+    <t>User is getting timesheet listing screen by clicking on "Back" button.</t>
+  </si>
+  <si>
+    <t>User should get screen for creating new timesheet entry by clicking on "New Entry" link.</t>
+  </si>
+  <si>
+    <t>User is getting screen for creating new timesheet entry by clicking on "New Entry" link.</t>
+  </si>
+  <si>
+    <t>User should get confirmation message by clicking on "Delete" option to delete particular timesheet entry.</t>
+  </si>
+  <si>
+    <t>User should get timesheet listing screen after successfully creating new timesheet.</t>
+  </si>
+  <si>
+    <t>User is getting timesheet listing screen after successfully creating new timesheet.</t>
+  </si>
+  <si>
+    <t>User should get timesheet listing by clicking on cancel button.</t>
+  </si>
+  <si>
+    <t>User is getting timesheet listing by clicking on cancel button.</t>
+  </si>
+  <si>
+    <t>User should get timesheet listing screen after successfully updating timesheet.</t>
+  </si>
+  <si>
+    <t>User is getting timesheet listing screen after successfully updating timesheet.</t>
+  </si>
+  <si>
+    <t>User should get timesheet listing screen by clicking on cancel button.</t>
+  </si>
+  <si>
+    <t>User is getting timesheet listing screen by clicking on cancel button.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -321,12 +322,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,118 +358,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C01345CA-536D-463E-83F8-35C114F8F294}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="9525"/>
-          <a:ext cx="8772524" cy="4200525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98DE3D0C-B444-4177-A419-6ED41E25C575}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1" y="1"/>
-          <a:ext cx="7153274" cy="4648200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9330855-B0B7-48A2-A614-F533C7645B35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90D87927-2075-4EF2-AD76-E184C655CF5C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -479,7 +388,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9248775" cy="3743325"/>
+          <a:ext cx="8562975" cy="3886200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -491,7 +400,56 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDF245F8-D9D0-4C4E-8856-D6A494E16CD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="0"/>
+          <a:ext cx="9029700" cy="4295775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -502,16 +460,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C95099E-92A1-4119-8BFF-D785A16DF6E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27883880-24C7-417C-AD49-84EEBD97F80C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -528,7 +486,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8410575" cy="4076700"/>
+          <a:ext cx="8334375" cy="4752975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -540,7 +498,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -550,17 +508,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>85214</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D550446-22A5-488E-926E-F4CBEB81E7C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71DA6475-0D6B-4928-8951-16F39A6BED52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -577,7 +535,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9077325" cy="4085714"/>
+          <a:ext cx="8353425" cy="3819525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -589,7 +547,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -947,390 +905,391 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="108.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" t="s">
         <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="C32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="C35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1339,7 +1298,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1313,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1328,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,11 +1339,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79B5B51-E58A-4A04-94C7-6F87F84B98B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B1F256-97B7-4536-B913-7112F0F3A3E7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,21 +1354,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B1F256-97B7-4536-B913-7112F0F3A3E7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C4F45B-612A-40F9-916A-1608B4592974}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>